<commit_message>
Page Speed insight-FCP & LCP
</commit_message>
<xml_diff>
--- a/src/test/Resources/TestData/PageSpeedOutput.xlsx
+++ b/src/test/Resources/TestData/PageSpeedOutput.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="334" uniqueCount="36">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="342" uniqueCount="36">
   <si>
     <t>Tvs Url</t>
   </si>
@@ -467,7 +467,7 @@
   <dimension ref="A1:F9"/>
   <sheetViews>
     <sheetView workbookViewId="0" tabSelected="true">
-      <selection activeCell="F9" sqref="F9"/>
+      <selection activeCell="D2" sqref="D2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.0"/>
@@ -475,8 +475,8 @@
     <col min="2" max="2" bestFit="true" customWidth="true" width="40.23828125"/>
     <col min="3" max="3" bestFit="true" customWidth="true" width="16.40625"/>
     <col min="4" max="4" bestFit="true" customWidth="true" width="16.0390625"/>
-    <col min="5" max="5" bestFit="true" customWidth="true" width="17.35546875"/>
-    <col min="6" max="6" bestFit="true" customWidth="true" width="16.98828125"/>
+    <col min="5" max="5" bestFit="true" customWidth="true" width="4.64453125"/>
+    <col min="6" max="6" bestFit="true" customWidth="true" width="4.64453125"/>
   </cols>
   <sheetData>
     <row r="1">
@@ -508,12 +508,6 @@
       <c r="D2" t="s" s="0">
         <v>11</v>
       </c>
-      <c r="E2" t="s" s="0">
-        <v>14</v>
-      </c>
-      <c r="F2" t="s" s="0">
-        <v>12</v>
-      </c>
     </row>
     <row r="3">
       <c r="A3" s="0"/>

</xml_diff>